<commit_message>
square fd when didn't need to; dG fixed
</commit_message>
<xml_diff>
--- a/2022_designAnalysisScripts/2022-11-20_gblock/2023-1-26_deltaGSummary.xlsx
+++ b/2022_designAnalysisScripts/2022-11-20_gblock/2023-1-26_deltaGSummary.xlsx
@@ -410,6 +410,11 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color rgb="FF595959"/>
       <name val="Calibri"/>
@@ -417,11 +422,6 @@
     </font>
     <font>
       <sz val="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -545,7 +545,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -730,69 +730,69 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>-4.10785855929946</c:v>
+                  <c:v>-4.61336706983439</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.96173303767245</c:v>
+                  <c:v>-3.14030060379344</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4.18837187869403</c:v>
+                  <c:v>-4.73156759834022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.44121419771987</c:v>
+                  <c:v>-3.71122941418482</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.79202289165066</c:v>
+                  <c:v>-4.16818986813174</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.49259270570967</c:v>
+                  <c:v>-3.77577483960995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-2.44969546751903</c:v>
+                  <c:v>-2.57212315872531</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.97855079641487</c:v>
+                  <c:v>-4.42735743282361</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.33969155001593</c:v>
+                  <c:v>-2.45327487734331</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-2.79339156191287</c:v>
+                  <c:v>-2.95010239286472</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-1.34776096498626</c:v>
+                  <c:v>-1.40440534564541</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-3.77956674140957</c:v>
+                  <c:v>-4.15128660810395</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-3.32510054204324</c:v>
+                  <c:v>-3.56806411550145</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-3.54777799768255</c:v>
+                  <c:v>-3.84597128416902</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-3.41235587858903</c:v>
+                  <c:v>-3.6753057764204</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-3.88058126135969</c:v>
+                  <c:v>-4.28983475783189</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-2.75635101630023</c:v>
+                  <c:v>-2.90876863626022</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-3.64024747590684</c:v>
+                  <c:v>-3.96569963940621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="36452456"/>
-        <c:axId val="1438322"/>
+        <c:axId val="19352425"/>
+        <c:axId val="88580217"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="36452456"/>
+        <c:axId val="19352425"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -834,12 +834,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1438322"/>
+        <c:crossAx val="88580217"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1438322"/>
+        <c:axId val="88580217"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,7 +881,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36452456"/>
+        <c:crossAx val="19352425"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -909,7 +909,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1064,39 +1064,39 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-4.10785855929946</c:v>
+                  <c:v>-4.61336706983439</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.96173303767245</c:v>
+                  <c:v>-3.14030060379344</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.79202289165066</c:v>
+                  <c:v>-4.16818986813174</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.49259270570967</c:v>
+                  <c:v>-3.77577483960995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.34776096498626</c:v>
+                  <c:v>-1.40440534564541</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.32510054204324</c:v>
+                  <c:v>-3.56806411550145</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.41235587858903</c:v>
+                  <c:v>-3.6753057764204</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.88058126135969</c:v>
+                  <c:v>-4.28983475783189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="99409607"/>
-        <c:axId val="44577795"/>
+        <c:axId val="8799494"/>
+        <c:axId val="9905596"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99409607"/>
+        <c:axId val="8799494"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1138,12 +1138,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44577795"/>
+        <c:crossAx val="9905596"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44577795"/>
+        <c:axId val="9905596"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1185,7 +1185,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99409607"/>
+        <c:crossAx val="8799494"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1213,7 +1213,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1374,45 +1374,45 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-4.18837187869403</c:v>
+                  <c:v>-4.73156759834022</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.44121419771987</c:v>
+                  <c:v>-3.71122941418482</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.44969546751903</c:v>
+                  <c:v>-2.57212315872531</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.97855079641487</c:v>
+                  <c:v>-4.42735743282361</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.33969155001593</c:v>
+                  <c:v>-2.45327487734331</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.79339156191287</c:v>
+                  <c:v>-2.95010239286472</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.77956674140957</c:v>
+                  <c:v>-4.15128660810395</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.54777799768255</c:v>
+                  <c:v>-3.84597128416902</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.75635101630023</c:v>
+                  <c:v>-2.90876863626022</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-3.64024747590684</c:v>
+                  <c:v>-3.96569963940621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2956493"/>
-        <c:axId val="8792929"/>
+        <c:axId val="35418625"/>
+        <c:axId val="58796900"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2956493"/>
+        <c:axId val="35418625"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1454,12 +1454,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8792929"/>
+        <c:crossAx val="58796900"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="8792929"/>
+        <c:axId val="58796900"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1501,7 +1501,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2956493"/>
+        <c:crossAx val="35418625"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1529,7 +1529,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1682,48 +1682,48 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-4.10785855929946</c:v>
+                  <c:v>-4.61336706983439</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.96173303767245</c:v>
+                  <c:v>-3.14030060379344</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4.18837187869403</c:v>
+                  <c:v>-4.73156759834022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.44121419771987</c:v>
+                  <c:v>-3.71122941418482</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.79202289165066</c:v>
+                  <c:v>-4.16818986813174</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.49259270570967</c:v>
+                  <c:v>-3.77577483960995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-2.44969546751903</c:v>
+                  <c:v>-2.57212315872531</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.97855079641487</c:v>
+                  <c:v>-4.42735743282361</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.33969155001593</c:v>
+                  <c:v>-2.45327487734331</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-2.79339156191287</c:v>
+                  <c:v>-2.95010239286472</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-1.34776096498626</c:v>
+                  <c:v>-1.40440534564541</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="66791253"/>
-        <c:axId val="32682229"/>
+        <c:axId val="38380621"/>
+        <c:axId val="15187620"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66791253"/>
+        <c:axId val="38380621"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1765,12 +1765,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32682229"/>
+        <c:crossAx val="15187620"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32682229"/>
+        <c:axId val="15187620"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1812,7 +1812,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66791253"/>
+        <c:crossAx val="38380621"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1840,7 +1840,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1981,36 +1981,36 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>-3.77956674140957</c:v>
+                  <c:v>-4.15128660810395</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.32510054204324</c:v>
+                  <c:v>-3.56806411550145</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.54777799768255</c:v>
+                  <c:v>-3.84597128416902</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.41235587858903</c:v>
+                  <c:v>-3.6753057764204</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.88058126135969</c:v>
+                  <c:v>-4.28983475783189</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.75635101630023</c:v>
+                  <c:v>-2.90876863626022</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.64024747590684</c:v>
+                  <c:v>-3.96569963940621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="51351270"/>
-        <c:axId val="98290636"/>
+        <c:axId val="72651341"/>
+        <c:axId val="77592209"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51351270"/>
+        <c:axId val="72651341"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2052,12 +2052,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98290636"/>
+        <c:crossAx val="77592209"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98290636"/>
+        <c:axId val="77592209"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2099,7 +2099,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51351270"/>
+        <c:crossAx val="72651341"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2127,7 +2127,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2262,30 +2262,30 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-4.10785855929946</c:v>
+                  <c:v>-4.61336706983439</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.96173303767245</c:v>
+                  <c:v>-3.14030060379344</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.79202289165066</c:v>
+                  <c:v>-4.16818986813174</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.49259270570967</c:v>
+                  <c:v>-3.77577483960995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.34776096498626</c:v>
+                  <c:v>-1.40440534564541</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="32328297"/>
-        <c:axId val="19013325"/>
+        <c:axId val="95504791"/>
+        <c:axId val="60376743"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="32328297"/>
+        <c:axId val="95504791"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2327,12 +2327,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19013325"/>
+        <c:crossAx val="60376743"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="19013325"/>
+        <c:axId val="60376743"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2374,7 +2374,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32328297"/>
+        <c:crossAx val="95504791"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2402,7 +2402,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2540,33 +2540,33 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-4.18837187869403</c:v>
+                  <c:v>-4.73156759834022</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.44121419771987</c:v>
+                  <c:v>-3.71122941418482</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.44969546751903</c:v>
+                  <c:v>-2.57212315872531</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.97855079641487</c:v>
+                  <c:v>-4.42735743282361</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.33969155001593</c:v>
+                  <c:v>-2.45327487734331</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.79339156191287</c:v>
+                  <c:v>-2.95010239286472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="71511293"/>
-        <c:axId val="19539040"/>
+        <c:axId val="5769637"/>
+        <c:axId val="31369868"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71511293"/>
+        <c:axId val="5769637"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2608,12 +2608,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19539040"/>
+        <c:crossAx val="31369868"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="19539040"/>
+        <c:axId val="31369868"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2655,7 +2655,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71511293"/>
+        <c:crossAx val="5769637"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2683,7 +2683,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2753,6 +2753,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2819,45 +2820,45 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-4.10785855929946</c:v>
+                  <c:v>-4.61336706983439</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.96173303767245</c:v>
+                  <c:v>-3.14030060379344</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4.18837187869403</c:v>
+                  <c:v>-4.73156759834022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.44121419771987</c:v>
+                  <c:v>-3.71122941418482</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.79202289165066</c:v>
+                  <c:v>-4.16818986813174</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.97855079641487</c:v>
+                  <c:v>-4.42735743282361</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.34776096498626</c:v>
+                  <c:v>-1.40440534564541</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.88058126135969</c:v>
+                  <c:v>-4.28983475783189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="84090581"/>
-        <c:axId val="85000257"/>
+        <c:axId val="67970570"/>
+        <c:axId val="18313491"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84090581"/>
+        <c:axId val="67970570"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2879,12 +2880,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85000257"/>
+        <c:crossAx val="18313491"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85000257"/>
+        <c:axId val="18313491"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2899,7 +2900,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2921,7 +2922,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84090581"/>
+        <c:crossAx val="67970570"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2941,14 +2942,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3018,6 +3019,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3086,51 +3088,51 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-3.49259270570967</c:v>
+                  <c:v>-3.77577483960995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.44969546751903</c:v>
+                  <c:v>-2.57212315872531</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.33969155001593</c:v>
+                  <c:v>-2.45327487734331</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.79339156191287</c:v>
+                  <c:v>-2.95010239286472</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.77956674140957</c:v>
+                  <c:v>-4.15128660810395</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.32510054204324</c:v>
+                  <c:v>-3.56806411550145</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.54777799768255</c:v>
+                  <c:v>-3.84597128416902</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.41235587858903</c:v>
+                  <c:v>-3.6753057764204</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.75635101630023</c:v>
+                  <c:v>-2.90876863626022</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-3.64024747590684</c:v>
+                  <c:v>-3.96569963940621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="3314619"/>
-        <c:axId val="46723623"/>
+        <c:axId val="53142155"/>
+        <c:axId val="69482907"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3314619"/>
+        <c:axId val="53142155"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3152,12 +3154,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46723623"/>
+        <c:crossAx val="69482907"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46723623"/>
+        <c:axId val="69482907"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3172,7 +3174,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3194,7 +3196,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3314619"/>
+        <c:crossAx val="53142155"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3214,7 +3216,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -3226,15 +3228,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>343080</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:colOff>397800</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>185040</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>30240</xdr:rowOff>
+      <xdr:colOff>239400</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>114480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3242,8 +3244,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="343080" y="12506760"/>
-        <a:ext cx="5306040" cy="2730240"/>
+        <a:off x="397800" y="12411000"/>
+        <a:ext cx="5309280" cy="2729880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3256,15 +3258,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>561960</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:colOff>562320</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>544320</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>136800</xdr:rowOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3272,8 +3274,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6026040" y="12427920"/>
-        <a:ext cx="5294160" cy="2730240"/>
+        <a:off x="6030000" y="12245400"/>
+        <a:ext cx="5298480" cy="2729880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3286,15 +3288,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>704160</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:colOff>704520</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>693360</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>81720</xdr:rowOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3302,8 +3304,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12238920" y="12372840"/>
-        <a:ext cx="5300640" cy="2730240"/>
+        <a:off x="12247920" y="12190320"/>
+        <a:ext cx="5305320" cy="2729880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3317,14 +3319,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3600</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>72000</xdr:rowOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>69840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>605520</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:colOff>605160</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>69120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3332,8 +3334,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3600" y="15649560"/>
-        <a:ext cx="5307120" cy="2781000"/>
+        <a:off x="3600" y="15467040"/>
+        <a:ext cx="5310000" cy="2780640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3346,15 +3348,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>443520</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>184320</xdr:rowOff>
+      <xdr:colOff>421920</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>73440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>425880</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>183960</xdr:rowOff>
+      <xdr:colOff>403920</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3362,8 +3364,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5907600" y="15576480"/>
-        <a:ext cx="5294160" cy="2781000"/>
+        <a:off x="5889600" y="15285240"/>
+        <a:ext cx="5298480" cy="2780640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3376,15 +3378,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>611280</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:colOff>611640</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>594000</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>9720</xdr:rowOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3392,8 +3394,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12146040" y="15587640"/>
-        <a:ext cx="5294160" cy="2781000"/>
+        <a:off x="12155040" y="15405120"/>
+        <a:ext cx="5298840" cy="2780640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3407,14 +3409,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>207360</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>35280</xdr:colOff>
-      <xdr:row>117</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:colOff>34920</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3422,8 +3424,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="207360" y="18750240"/>
-        <a:ext cx="5292000" cy="2781360"/>
+        <a:off x="207360" y="18567720"/>
+        <a:ext cx="5295240" cy="2781000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3436,15 +3438,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>233280</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>173520</xdr:rowOff>
+      <xdr:colOff>233640</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>681120</xdr:colOff>
-      <xdr:row>119</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>73080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3452,8 +3454,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5697360" y="18717840"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="5701320" y="18535320"/>
+        <a:ext cx="5763960" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3466,15 +3468,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>233280</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:colOff>233640</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>681480</xdr:colOff>
-      <xdr:row>119</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>88200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3482,8 +3484,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11768040" y="18732960"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="11777040" y="18550440"/>
+        <a:ext cx="5764320" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3503,11 +3505,11 @@
   </sheetPr>
   <dimension ref="A1:X63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P75" activeCellId="0" sqref="P75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y106" activeCellId="0" sqref="Y106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.25"/>
   </cols>
@@ -3583,7 +3585,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>0</v>
       </c>
@@ -3651,13 +3653,13 @@
         <v>0.308122796992481</v>
       </c>
       <c r="W2" s="0" t="n">
-        <v>0.000980695214511831</v>
+        <v>0.000559289558374183</v>
       </c>
       <c r="X2" s="0" t="n">
-        <v>-4.10785855929946</v>
+        <v>-4.61336706983439</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
@@ -3725,13 +3727,13 @@
         <v>0.0528462542173615</v>
       </c>
       <c r="W3" s="0" t="n">
-        <v>0.00677517021426608</v>
+        <v>0.0061112387872503</v>
       </c>
       <c r="X3" s="0" t="n">
-        <v>-2.96173303767245</v>
+        <v>-3.14030060379344</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -3799,13 +3801,13 @@
         <v>0.339847529733424</v>
       </c>
       <c r="W4" s="0" t="n">
-        <v>0.000856187025575942</v>
+        <v>0.000461643674040312</v>
       </c>
       <c r="X4" s="0" t="n">
-        <v>-4.18837187869403</v>
+        <v>-4.73156759834022</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -3870,13 +3872,13 @@
         <v>0.116236535912508</v>
       </c>
       <c r="W5" s="0" t="n">
-        <v>0.00301830653357823</v>
+        <v>0.00241897805674261</v>
       </c>
       <c r="X5" s="0" t="n">
-        <v>-3.44121419771987</v>
+        <v>-3.71122941418482</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
@@ -3941,13 +3943,13 @@
         <v>0.199991304989747</v>
       </c>
       <c r="W6" s="0" t="n">
-        <v>0.00167048326684769</v>
+        <v>0.00115207512829088</v>
       </c>
       <c r="X6" s="0" t="n">
-        <v>-3.79202289165066</v>
+        <v>-4.16818986813174</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
@@ -4015,13 +4017,13 @@
         <v>0.126186242105263</v>
       </c>
       <c r="W7" s="0" t="n">
-        <v>0.00276780408732288</v>
+        <v>0.00217835296042578</v>
       </c>
       <c r="X7" s="0" t="n">
-        <v>-3.49259270570967</v>
+        <v>-3.77577483960995</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
@@ -4089,13 +4091,13 @@
         <v>0.0223847148051947</v>
       </c>
       <c r="W8" s="0" t="n">
-        <v>0.0160664661898124</v>
+        <v>0.0153704612946376</v>
       </c>
       <c r="X8" s="0" t="n">
-        <v>-2.44969546751903</v>
+        <v>-2.57212315872531</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
@@ -4163,13 +4165,13 @@
         <v>0.260359279289131</v>
       </c>
       <c r="W9" s="0" t="n">
-        <v>0.00121964932568392</v>
+        <v>0.000756434043763887</v>
       </c>
       <c r="X9" s="0" t="n">
-        <v>-3.97855079641487</v>
+        <v>-4.42735743282361</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
@@ -4237,13 +4239,13 @@
         <v>0.0186003417634996</v>
       </c>
       <c r="W10" s="0" t="n">
-        <v>0.0193412153871248</v>
+        <v>0.0186411792060525</v>
       </c>
       <c r="X10" s="0" t="n">
-        <v>-2.33969155001593</v>
+        <v>-2.45327487734331</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
@@ -4308,13 +4310,13 @@
         <v>0.0398784642515379</v>
       </c>
       <c r="W11" s="0" t="n">
-        <v>0.00899928889397692</v>
+        <v>0.0083217851302806</v>
       </c>
       <c r="X11" s="0" t="n">
-        <v>-2.79339156191287</v>
+        <v>-2.95010239286472</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
@@ -4379,13 +4381,13 @@
         <v>0.00349421402597403</v>
       </c>
       <c r="W12" s="0" t="n">
-        <v>0.103024949765472</v>
+        <v>0.102308719121189</v>
       </c>
       <c r="X12" s="0" t="n">
-        <v>-1.34776096498626</v>
+        <v>-1.40440534564541</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
@@ -4453,13 +4455,13 @@
         <v>0.196352464798359</v>
       </c>
       <c r="W13" s="0" t="n">
-        <v>0.00170594341159123</v>
+        <v>0.0011841245290178</v>
       </c>
       <c r="X13" s="0" t="n">
-        <v>-3.77956674140957</v>
+        <v>-4.15128660810395</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
@@ -4527,13 +4529,13 @@
         <v>0.0963298323718386</v>
       </c>
       <c r="W14" s="0" t="n">
-        <v>0.00367114315579448</v>
+        <v>0.00305183877757835</v>
       </c>
       <c r="X14" s="0" t="n">
-        <v>-3.32510054204324</v>
+        <v>-3.56806411550145</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
@@ -4601,13 +4603,13 @@
         <v>0.1377107316473</v>
       </c>
       <c r="W15" s="0" t="n">
-        <v>0.00252185075088708</v>
+        <v>0.00194375121264627</v>
       </c>
       <c r="X15" s="0" t="n">
-        <v>-3.54777799768255</v>
+        <v>-3.84597128416902</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
@@ -4675,13 +4677,13 @@
         <v>0.110964300451127</v>
       </c>
       <c r="W16" s="0" t="n">
-        <v>0.0031688250738213</v>
+        <v>0.00256423381095767</v>
       </c>
       <c r="X16" s="0" t="n">
-        <v>-3.41235587858903</v>
+        <v>-3.6753057764204</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
@@ -4749,13 +4751,13 @@
         <v>0.227300705399863</v>
       </c>
       <c r="W17" s="0" t="n">
-        <v>0.00143874813960213</v>
+        <v>0.000945633281590893</v>
       </c>
       <c r="X17" s="0" t="n">
-        <v>-3.88058126135969</v>
+        <v>-4.28983475783189</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
@@ -4823,13 +4825,13 @@
         <v>0.0374772929870129</v>
       </c>
       <c r="W18" s="0" t="n">
-        <v>0.00957933850348989</v>
+        <v>0.0088993083428196</v>
       </c>
       <c r="X18" s="0" t="n">
-        <v>-2.75635101630023</v>
+        <v>-2.90876863626022</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
@@ -4894,10 +4896,10 @@
         <v>0.159070041203007</v>
       </c>
       <c r="W19" s="0" t="n">
-        <v>0.00215773275023608</v>
+        <v>0.00160041921465234</v>
       </c>
       <c r="X19" s="0" t="n">
-        <v>-3.64024747590684</v>
+        <v>-3.96569963940621</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4974,7 +4976,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>0</v>
       </c>
@@ -5042,13 +5044,13 @@
         <v>0.308122796992481</v>
       </c>
       <c r="W22" s="0" t="n">
-        <v>0.000980695214511831</v>
+        <v>0.000559289558374183</v>
       </c>
       <c r="X22" s="0" t="n">
-        <v>-4.10785855929946</v>
+        <v>-4.61336706983439</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>1</v>
       </c>
@@ -5116,13 +5118,13 @@
         <v>0.0528462542173615</v>
       </c>
       <c r="W23" s="0" t="n">
-        <v>0.00677517021426608</v>
+        <v>0.0061112387872503</v>
       </c>
       <c r="X23" s="0" t="n">
-        <v>-2.96173303767245</v>
+        <v>-3.14030060379344</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>5</v>
       </c>
@@ -5187,13 +5189,13 @@
         <v>0.199991304989747</v>
       </c>
       <c r="W24" s="0" t="n">
-        <v>0.00167048326684769</v>
+        <v>0.00115207512829088</v>
       </c>
       <c r="X24" s="0" t="n">
-        <v>-3.79202289165066</v>
+        <v>-4.16818986813174</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>6</v>
       </c>
@@ -5261,13 +5263,13 @@
         <v>0.126186242105263</v>
       </c>
       <c r="W25" s="0" t="n">
-        <v>0.00276780408732288</v>
+        <v>0.00217835296042578</v>
       </c>
       <c r="X25" s="0" t="n">
-        <v>-3.49259270570967</v>
+        <v>-3.77577483960995</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>11</v>
       </c>
@@ -5332,13 +5334,13 @@
         <v>0.00349421402597403</v>
       </c>
       <c r="W26" s="0" t="n">
-        <v>0.103024949765472</v>
+        <v>0.102308719121189</v>
       </c>
       <c r="X26" s="0" t="n">
-        <v>-1.34776096498626</v>
+        <v>-1.40440534564541</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>13</v>
       </c>
@@ -5406,13 +5408,13 @@
         <v>0.0963298323718386</v>
       </c>
       <c r="W27" s="0" t="n">
-        <v>0.00367114315579448</v>
+        <v>0.00305183877757835</v>
       </c>
       <c r="X27" s="0" t="n">
-        <v>-3.32510054204324</v>
+        <v>-3.56806411550145</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>15</v>
       </c>
@@ -5480,13 +5482,13 @@
         <v>0.110964300451127</v>
       </c>
       <c r="W28" s="0" t="n">
-        <v>0.0031688250738213</v>
+        <v>0.00256423381095767</v>
       </c>
       <c r="X28" s="0" t="n">
-        <v>-3.41235587858903</v>
+        <v>-3.6753057764204</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>16</v>
       </c>
@@ -5554,10 +5556,10 @@
         <v>0.227300705399863</v>
       </c>
       <c r="W29" s="0" t="n">
-        <v>0.00143874813960213</v>
+        <v>0.000945633281590893</v>
       </c>
       <c r="X29" s="0" t="n">
-        <v>-3.88058126135969</v>
+        <v>-4.28983475783189</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5634,7 +5636,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>3</v>
       </c>
@@ -5702,13 +5704,13 @@
         <v>0.339847529733424</v>
       </c>
       <c r="W32" s="0" t="n">
-        <v>0.000856187025575942</v>
+        <v>0.000461643674040312</v>
       </c>
       <c r="X32" s="0" t="n">
-        <v>-4.18837187869403</v>
+        <v>-4.73156759834022</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>4</v>
       </c>
@@ -5773,13 +5775,13 @@
         <v>0.116236535912508</v>
       </c>
       <c r="W33" s="0" t="n">
-        <v>0.00301830653357823</v>
+        <v>0.00241897805674261</v>
       </c>
       <c r="X33" s="0" t="n">
-        <v>-3.44121419771987</v>
+        <v>-3.71122941418482</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>7</v>
       </c>
@@ -5847,13 +5849,13 @@
         <v>0.0223847148051947</v>
       </c>
       <c r="W34" s="0" t="n">
-        <v>0.0160664661898124</v>
+        <v>0.0153704612946376</v>
       </c>
       <c r="X34" s="0" t="n">
-        <v>-2.44969546751903</v>
+        <v>-2.57212315872531</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>8</v>
       </c>
@@ -5921,13 +5923,13 @@
         <v>0.260359279289131</v>
       </c>
       <c r="W35" s="0" t="n">
-        <v>0.00121964932568392</v>
+        <v>0.000756434043763887</v>
       </c>
       <c r="X35" s="0" t="n">
-        <v>-3.97855079641487</v>
+        <v>-4.42735743282361</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>9</v>
       </c>
@@ -5995,13 +5997,13 @@
         <v>0.0186003417634996</v>
       </c>
       <c r="W36" s="0" t="n">
-        <v>0.0193412153871248</v>
+        <v>0.0186411792060525</v>
       </c>
       <c r="X36" s="0" t="n">
-        <v>-2.33969155001593</v>
+        <v>-2.45327487734331</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>10</v>
       </c>
@@ -6066,13 +6068,13 @@
         <v>0.0398784642515379</v>
       </c>
       <c r="W37" s="0" t="n">
-        <v>0.00899928889397692</v>
+        <v>0.0083217851302806</v>
       </c>
       <c r="X37" s="0" t="n">
-        <v>-2.79339156191287</v>
+        <v>-2.95010239286472</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>12</v>
       </c>
@@ -6140,13 +6142,13 @@
         <v>0.196352464798359</v>
       </c>
       <c r="W38" s="0" t="n">
-        <v>0.00170594341159123</v>
+        <v>0.0011841245290178</v>
       </c>
       <c r="X38" s="0" t="n">
-        <v>-3.77956674140957</v>
+        <v>-4.15128660810395</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>14</v>
       </c>
@@ -6214,13 +6216,13 @@
         <v>0.1377107316473</v>
       </c>
       <c r="W39" s="0" t="n">
-        <v>0.00252185075088708</v>
+        <v>0.00194375121264627</v>
       </c>
       <c r="X39" s="0" t="n">
-        <v>-3.54777799768255</v>
+        <v>-3.84597128416902</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>17</v>
       </c>
@@ -6288,13 +6290,13 @@
         <v>0.0374772929870129</v>
       </c>
       <c r="W40" s="0" t="n">
-        <v>0.00957933850348989</v>
+        <v>0.0088993083428196</v>
       </c>
       <c r="X40" s="0" t="n">
-        <v>-2.75635101630023</v>
+        <v>-2.90876863626022</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>18</v>
       </c>
@@ -6359,10 +6361,10 @@
         <v>0.159070041203007</v>
       </c>
       <c r="W41" s="0" t="n">
-        <v>0.00215773275023608</v>
+        <v>0.00160041921465234</v>
       </c>
       <c r="X41" s="0" t="n">
-        <v>-3.64024747590684</v>
+        <v>-3.96569963940621</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6507,10 +6509,10 @@
         <v>0.308122796992481</v>
       </c>
       <c r="W44" s="0" t="n">
-        <v>0.000980695214511831</v>
+        <v>0.000559289558374183</v>
       </c>
       <c r="X44" s="0" t="n">
-        <v>-4.10785855929946</v>
+        <v>-4.61336706983439</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6581,10 +6583,10 @@
         <v>0.0528462542173615</v>
       </c>
       <c r="W45" s="0" t="n">
-        <v>0.00677517021426608</v>
+        <v>0.0061112387872503</v>
       </c>
       <c r="X45" s="0" t="n">
-        <v>-2.96173303767245</v>
+        <v>-3.14030060379344</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6655,10 +6657,10 @@
         <v>0.339847529733424</v>
       </c>
       <c r="W46" s="0" t="n">
-        <v>0.000856187025575942</v>
+        <v>0.000461643674040312</v>
       </c>
       <c r="X46" s="0" t="n">
-        <v>-4.18837187869403</v>
+        <v>-4.73156759834022</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6726,10 +6728,10 @@
         <v>0.116236535912508</v>
       </c>
       <c r="W47" s="0" t="n">
-        <v>0.00301830653357823</v>
+        <v>0.00241897805674261</v>
       </c>
       <c r="X47" s="0" t="n">
-        <v>-3.44121419771987</v>
+        <v>-3.71122941418482</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6797,10 +6799,10 @@
         <v>0.199991304989747</v>
       </c>
       <c r="W48" s="0" t="n">
-        <v>0.00167048326684769</v>
+        <v>0.00115207512829088</v>
       </c>
       <c r="X48" s="0" t="n">
-        <v>-3.79202289165066</v>
+        <v>-4.16818986813174</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6871,10 +6873,10 @@
         <v>0.260359279289131</v>
       </c>
       <c r="W49" s="0" t="n">
-        <v>0.00121964932568392</v>
+        <v>0.000756434043763887</v>
       </c>
       <c r="X49" s="0" t="n">
-        <v>-3.97855079641487</v>
+        <v>-4.42735743282361</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6942,10 +6944,10 @@
         <v>0.00349421402597403</v>
       </c>
       <c r="W50" s="0" t="n">
-        <v>0.103024949765472</v>
+        <v>0.102308719121189</v>
       </c>
       <c r="X50" s="0" t="n">
-        <v>-1.34776096498626</v>
+        <v>-1.40440534564541</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7016,10 +7018,10 @@
         <v>0.227300705399863</v>
       </c>
       <c r="W51" s="0" t="n">
-        <v>0.00143874813960213</v>
+        <v>0.000945633281590893</v>
       </c>
       <c r="X51" s="0" t="n">
-        <v>-3.88058126135969</v>
+        <v>-4.28983475783189</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7164,10 +7166,10 @@
         <v>0.126186242105263</v>
       </c>
       <c r="W54" s="0" t="n">
-        <v>0.00276780408732288</v>
+        <v>0.00217835296042578</v>
       </c>
       <c r="X54" s="0" t="n">
-        <v>-3.49259270570967</v>
+        <v>-3.77577483960995</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7238,10 +7240,10 @@
         <v>0.0223847148051947</v>
       </c>
       <c r="W55" s="0" t="n">
-        <v>0.0160664661898124</v>
+        <v>0.0153704612946376</v>
       </c>
       <c r="X55" s="0" t="n">
-        <v>-2.44969546751903</v>
+        <v>-2.57212315872531</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7312,10 +7314,10 @@
         <v>0.0186003417634996</v>
       </c>
       <c r="W56" s="0" t="n">
-        <v>0.0193412153871248</v>
+        <v>0.0186411792060525</v>
       </c>
       <c r="X56" s="0" t="n">
-        <v>-2.33969155001593</v>
+        <v>-2.45327487734331</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7383,10 +7385,10 @@
         <v>0.0398784642515379</v>
       </c>
       <c r="W57" s="0" t="n">
-        <v>0.00899928889397692</v>
+        <v>0.0083217851302806</v>
       </c>
       <c r="X57" s="0" t="n">
-        <v>-2.79339156191287</v>
+        <v>-2.95010239286472</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7457,10 +7459,10 @@
         <v>0.196352464798359</v>
       </c>
       <c r="W58" s="0" t="n">
-        <v>0.00170594341159123</v>
+        <v>0.0011841245290178</v>
       </c>
       <c r="X58" s="0" t="n">
-        <v>-3.77956674140957</v>
+        <v>-4.15128660810395</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7531,10 +7533,10 @@
         <v>0.0963298323718386</v>
       </c>
       <c r="W59" s="0" t="n">
-        <v>0.00367114315579448</v>
+        <v>0.00305183877757835</v>
       </c>
       <c r="X59" s="0" t="n">
-        <v>-3.32510054204324</v>
+        <v>-3.56806411550145</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7605,10 +7607,10 @@
         <v>0.1377107316473</v>
       </c>
       <c r="W60" s="0" t="n">
-        <v>0.00252185075088708</v>
+        <v>0.00194375121264627</v>
       </c>
       <c r="X60" s="0" t="n">
-        <v>-3.54777799768255</v>
+        <v>-3.84597128416902</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7679,10 +7681,10 @@
         <v>0.110964300451127</v>
       </c>
       <c r="W61" s="0" t="n">
-        <v>0.0031688250738213</v>
+        <v>0.00256423381095767</v>
       </c>
       <c r="X61" s="0" t="n">
-        <v>-3.41235587858903</v>
+        <v>-3.6753057764204</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7753,10 +7755,10 @@
         <v>0.0374772929870129</v>
       </c>
       <c r="W62" s="0" t="n">
-        <v>0.00957933850348989</v>
+        <v>0.0088993083428196</v>
       </c>
       <c r="X62" s="0" t="n">
-        <v>-2.75635101630023</v>
+        <v>-2.90876863626022</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7824,10 +7826,10 @@
         <v>0.159070041203007</v>
       </c>
       <c r="W63" s="0" t="n">
-        <v>0.00215773275023608</v>
+        <v>0.00160041921465234</v>
       </c>
       <c r="X63" s="0" t="n">
-        <v>-3.64024747590684</v>
+        <v>-3.96569963940621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with JC data
</commit_message>
<xml_diff>
--- a/2022_designAnalysisScripts/2022-11-20_gblock/2023-1-26_deltaGSummary.xlsx
+++ b/2022_designAnalysisScripts/2022-11-20_gblock/2023-1-26_deltaGSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gjowl\github\Sequence-Design\2022_designAnalysisScripts\2022-11-20_gblock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD6F72A-43E0-4F87-9BCA-3F512DEAAEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E42DAF-BCD9-4A31-B29A-CF5E41635D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="113">
   <si>
     <t>Design</t>
   </si>
@@ -344,6 +344,27 @@
   <si>
     <t>No Hbond</t>
   </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>JC Data + right</t>
+  </si>
+  <si>
+    <t>JC Data + hbond</t>
+  </si>
 </sst>
 </file>
 
@@ -839,6 +860,1307 @@
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>deltaG right + Josh Designs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.58059011373578306"/>
+                  <c:y val="-0.37831583552055992"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>test!$D$58:$D$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-18.1389</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-38.856699999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-21.300599999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-40.000900000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-46.956899999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-33.175899999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-42.155999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-46.848999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-7.9169700000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-18.024000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-24.5886</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-12.117599999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>test!$K$58:$K$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-2.6301268021156901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.1083984846542503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.2671951829985</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.5966021411261098</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.61336706983439</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.14030060379344</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.7315675983402201</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-4.1681898681317398</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-3.7757748396099502</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2.5721231587253102</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2.45327487734331</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.40440534564541</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CC4-4D72-9E9D-9629E36E7D36}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="674576847"/>
+        <c:axId val="674563535"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="674576847"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="674563535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="674563535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="674576847"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>deltaG + Josh Design (hbond only)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.50362926509186356"/>
+                  <c:y val="-0.31838910761154854"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>test!$P$58:$P$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-38.856699999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-40.000900000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-46.956899999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-33.175899999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-42.155999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-46.848999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-12.117599999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-36.766300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>test!$W$58:$W$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-5.1083984846542503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.5966021411261098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.61336706983439</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.14030060379344</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.7315675983402201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.1681898681317398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.40440534564541</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-4.2898347578318896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6628-4FB3-BA21-C23E10F6052F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="820505759"/>
+        <c:axId val="820507423"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="820505759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="820507423"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="820507423"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="820505759"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>deltaG + Josh</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Designs (no hbnod)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.47623797025371828"/>
+                  <c:y val="-0.73750692621755609"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>test!$D$73:$D$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-18.1389</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-21.300599999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-7.9169700000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-18.024000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-24.5886</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-22.721900000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-19.871200000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-14.2117</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-17.953700000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-18.429099999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-23.184699999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>test!$K$73:$K$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-2.6301268021156901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.2671951829985</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.7757748396099502</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.5721231587253102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.45327487734331</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.1512866081039501</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-3.5680641155014499</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3.8459712841690199</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-3.6753057764203998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2.9087686362602199</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.9656996394062101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9E20-49A3-B53D-2B7C96297F6D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="820485791"/>
+        <c:axId val="820473311"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="820485791"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="820473311"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="820473311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="820485791"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -3377,20 +4699,1688 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>313133</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>55893</xdr:rowOff>
+      <xdr:colOff>309533</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>149030</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>154733</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>4413</xdr:rowOff>
+      <xdr:colOff>151133</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>97550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3417,16 +6407,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>562320</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>33787</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>42696</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>544320</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>134280</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>15787</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>176616</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3453,16 +6443,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>704520</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>2420</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>12148</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>2480</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>583080</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>146935</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3490,15 +6480,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3600</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>86776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>5720</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
+      <xdr:colOff>2120</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>86056</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3526,15 +6516,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>421920</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:colOff>443720</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>22642</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>403920</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>72720</xdr:rowOff>
+      <xdr:colOff>425720</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>21922</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3561,16 +6551,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>611640</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>980</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>7924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>2180</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>7200</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>582780</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>7204</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3598,15 +6588,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>207360</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
+      <xdr:colOff>203760</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>35296</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>34920</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:colOff>31320</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>34936</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3634,15 +6624,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>233640</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:colOff>230040</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>2029</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>5480</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>73080</xdr:rowOff>
+      <xdr:colOff>1880</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>90016</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3670,15 +6660,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>233640</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:colOff>230040</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>18018</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>5840</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>88200</xdr:rowOff>
+      <xdr:colOff>2240</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>105137</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3698,6 +6688,114 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>233467</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>122768</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>13334</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>71968</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82A4CEA5-9A03-FBD9-2D95-4A5DE8E7FEDF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>411268</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>55034</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>309668</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>4235</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37827F2F-A086-0F3E-2645-4CF87C1DAEC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55B50FBB-5A3B-67F2-D842-3F2245BCA065}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4003,10 +7101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X54"/>
+  <dimension ref="A1:X83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="L131" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S139" sqref="S139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7684,9 +10782,1164 @@
         <v>-3.9656996394062101</v>
       </c>
     </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>111</v>
+      </c>
+      <c r="M56" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" t="s">
+        <v>10</v>
+      </c>
+      <c r="H57" t="s">
+        <v>19</v>
+      </c>
+      <c r="I57" t="s">
+        <v>20</v>
+      </c>
+      <c r="J57" t="s">
+        <v>21</v>
+      </c>
+      <c r="K57" t="s">
+        <v>22</v>
+      </c>
+      <c r="N57" t="s">
+        <v>106</v>
+      </c>
+      <c r="O57" t="s">
+        <v>5</v>
+      </c>
+      <c r="P57" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>8</v>
+      </c>
+      <c r="R57" t="s">
+        <v>9</v>
+      </c>
+      <c r="S57" t="s">
+        <v>10</v>
+      </c>
+      <c r="T57" t="s">
+        <v>19</v>
+      </c>
+      <c r="U57" t="s">
+        <v>20</v>
+      </c>
+      <c r="V57" t="s">
+        <v>21</v>
+      </c>
+      <c r="W57" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58">
+        <v>39.726865452189699</v>
+      </c>
+      <c r="D58">
+        <v>-18.1389</v>
+      </c>
+      <c r="E58">
+        <v>-36.149700000000003</v>
+      </c>
+      <c r="F58">
+        <v>5.0800000000009497E-2</v>
+      </c>
+      <c r="G58">
+        <v>17.96</v>
+      </c>
+      <c r="H58">
+        <v>33.042604956536003</v>
+      </c>
+      <c r="I58">
+        <v>2.4489037463266399E-2</v>
+      </c>
+      <c r="J58">
+        <v>1.3989271330261101E-2</v>
+      </c>
+      <c r="K58">
+        <v>-2.6301268021156901</v>
+      </c>
+      <c r="M58">
+        <v>1</v>
+      </c>
+      <c r="N58" t="s">
+        <v>108</v>
+      </c>
+      <c r="O58">
+        <v>193.223909124941</v>
+      </c>
+      <c r="P58">
+        <v>-38.856699999999996</v>
+      </c>
+      <c r="Q58">
+        <v>-54.440300000000001</v>
+      </c>
+      <c r="R58">
+        <v>-4.8799000000000001</v>
+      </c>
+      <c r="S58">
+        <v>20.463999999999999</v>
+      </c>
+      <c r="T58">
+        <v>172.585371931764</v>
+      </c>
+      <c r="U58">
+        <v>0.44416653212560703</v>
+      </c>
+      <c r="V58">
+        <v>2.50406763677289E-4</v>
+      </c>
+      <c r="W58">
+        <v>-5.1083984846542503</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59">
+        <v>193.223909124941</v>
+      </c>
+      <c r="D59">
+        <v>-38.856699999999996</v>
+      </c>
+      <c r="E59">
+        <v>-54.440300000000001</v>
+      </c>
+      <c r="F59">
+        <v>-4.8799000000000001</v>
+      </c>
+      <c r="G59">
+        <v>20.463999999999999</v>
+      </c>
+      <c r="H59">
+        <v>172.585371931764</v>
+      </c>
+      <c r="I59">
+        <v>0.44416653212560703</v>
+      </c>
+      <c r="J59">
+        <v>2.50406763677289E-4</v>
+      </c>
+      <c r="K59">
+        <v>-5.1083984846542503</v>
+      </c>
+      <c r="M59">
+        <v>3</v>
+      </c>
+      <c r="N59" t="s">
+        <v>110</v>
+      </c>
+      <c r="O59">
+        <v>141.84755549832599</v>
+      </c>
+      <c r="P59">
+        <v>-40.000900000000001</v>
+      </c>
+      <c r="Q59">
+        <v>-48.1464</v>
+      </c>
+      <c r="R59">
+        <v>-11.3764</v>
+      </c>
+      <c r="S59">
+        <v>19.521999999999998</v>
+      </c>
+      <c r="T59">
+        <v>125.879595907569</v>
+      </c>
+      <c r="U59">
+        <v>0.30369803280471802</v>
+      </c>
+      <c r="V59">
+        <v>5.74719279592562E-4</v>
+      </c>
+      <c r="W59">
+        <v>-4.5966021411261098</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>2</v>
+      </c>
+      <c r="B60" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60">
+        <v>53.989196811001698</v>
+      </c>
+      <c r="D60">
+        <v>-21.300599999999999</v>
+      </c>
+      <c r="E60">
+        <v>-44.918700000000001</v>
+      </c>
+      <c r="F60">
+        <v>0.201399999999992</v>
+      </c>
+      <c r="G60">
+        <v>23.417000000000002</v>
+      </c>
+      <c r="H60">
+        <v>46.008360737274202</v>
+      </c>
+      <c r="I60">
+        <v>6.3483791691050395E-2</v>
+      </c>
+      <c r="J60">
+        <v>4.9735929537687799E-3</v>
+      </c>
+      <c r="K60">
+        <v>-3.2671951829985</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60" t="s">
+        <v>26</v>
+      </c>
+      <c r="O60">
+        <v>143.465913</v>
+      </c>
+      <c r="P60">
+        <v>-46.956899999999997</v>
+      </c>
+      <c r="Q60">
+        <v>-43.674599999999998</v>
+      </c>
+      <c r="R60">
+        <v>-30.256900000000002</v>
+      </c>
+      <c r="S60">
+        <v>26.975000000000001</v>
+      </c>
+      <c r="T60">
+        <v>127.35082999999899</v>
+      </c>
+      <c r="U60">
+        <v>0.30812279699248102</v>
+      </c>
+      <c r="V60">
+        <v>5.5928955837418297E-4</v>
+      </c>
+      <c r="W60">
+        <v>-4.61336706983439</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61">
+        <v>141.84755549832599</v>
+      </c>
+      <c r="D61">
+        <v>-40.000900000000001</v>
+      </c>
+      <c r="E61">
+        <v>-48.1464</v>
+      </c>
+      <c r="F61">
+        <v>-11.3764</v>
+      </c>
+      <c r="G61">
+        <v>19.521999999999998</v>
+      </c>
+      <c r="H61">
+        <v>125.879595907569</v>
+      </c>
+      <c r="I61">
+        <v>0.30369803280471802</v>
+      </c>
+      <c r="J61">
+        <v>5.74719279592562E-4</v>
+      </c>
+      <c r="K61">
+        <v>-4.5966021411261098</v>
+      </c>
+      <c r="M61">
+        <v>1</v>
+      </c>
+      <c r="N61" t="s">
+        <v>33</v>
+      </c>
+      <c r="O61">
+        <v>50.098517479999998</v>
+      </c>
+      <c r="P61">
+        <v>-33.175899999999999</v>
+      </c>
+      <c r="Q61">
+        <v>-40.406199999999998</v>
+      </c>
+      <c r="R61">
+        <v>-24.622599999999998</v>
+      </c>
+      <c r="S61">
+        <v>31.853000000000002</v>
+      </c>
+      <c r="T61">
+        <v>42.471379527272703</v>
+      </c>
+      <c r="U61">
+        <v>5.2846254217361499E-2</v>
+      </c>
+      <c r="V61">
+        <v>6.1112387872503003E-3</v>
+      </c>
+      <c r="W61">
+        <v>-3.14030060379344</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62">
+        <v>143.465913</v>
+      </c>
+      <c r="D62">
+        <v>-46.956899999999997</v>
+      </c>
+      <c r="E62">
+        <v>-43.674599999999998</v>
+      </c>
+      <c r="F62">
+        <v>-30.256900000000002</v>
+      </c>
+      <c r="G62">
+        <v>26.975000000000001</v>
+      </c>
+      <c r="H62">
+        <v>127.35082999999899</v>
+      </c>
+      <c r="I62">
+        <v>0.30812279699248102</v>
+      </c>
+      <c r="J62">
+        <v>5.5928955837418297E-4</v>
+      </c>
+      <c r="K62">
+        <v>-4.61336706983439</v>
+      </c>
+      <c r="M62">
+        <v>3</v>
+      </c>
+      <c r="N62" t="s">
+        <v>38</v>
+      </c>
+      <c r="O62">
+        <v>155.06923399999999</v>
+      </c>
+      <c r="P62">
+        <v>-42.155999999999999</v>
+      </c>
+      <c r="Q62">
+        <v>-50.616900000000001</v>
+      </c>
+      <c r="R62">
+        <v>-12.7387</v>
+      </c>
+      <c r="S62">
+        <v>21.2</v>
+      </c>
+      <c r="T62">
+        <v>137.89930363636299</v>
+      </c>
+      <c r="U62">
+        <v>0.33984752973342403</v>
+      </c>
+      <c r="V62">
+        <v>4.6164367404031198E-4</v>
+      </c>
+      <c r="W62">
+        <v>-4.7315675983402201</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63">
+        <v>50.098517479999998</v>
+      </c>
+      <c r="D63">
+        <v>-33.175899999999999</v>
+      </c>
+      <c r="E63">
+        <v>-40.406199999999998</v>
+      </c>
+      <c r="F63">
+        <v>-24.622599999999998</v>
+      </c>
+      <c r="G63">
+        <v>31.853000000000002</v>
+      </c>
+      <c r="H63">
+        <v>42.471379527272703</v>
+      </c>
+      <c r="I63">
+        <v>5.2846254217361499E-2</v>
+      </c>
+      <c r="J63">
+        <v>6.1112387872503003E-3</v>
+      </c>
+      <c r="K63">
+        <v>-3.14030060379344</v>
+      </c>
+      <c r="M63">
+        <v>5</v>
+      </c>
+      <c r="N63" t="s">
+        <v>44</v>
+      </c>
+      <c r="O63">
+        <v>103.9168198</v>
+      </c>
+      <c r="P63">
+        <v>-46.848999999999997</v>
+      </c>
+      <c r="Q63">
+        <v>-63.137799999999999</v>
+      </c>
+      <c r="R63">
+        <v>-7.4077000000000002</v>
+      </c>
+      <c r="S63">
+        <v>23.696000000000002</v>
+      </c>
+      <c r="T63">
+        <v>91.397108909090903</v>
+      </c>
+      <c r="U63">
+        <v>0.19999130498974699</v>
+      </c>
+      <c r="V63">
+        <v>1.1520751282908801E-3</v>
+      </c>
+      <c r="W63">
+        <v>-4.1681898681317398</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>3</v>
+      </c>
+      <c r="B64" t="s">
+        <v>38</v>
+      </c>
+      <c r="C64">
+        <v>155.06923399999999</v>
+      </c>
+      <c r="D64">
+        <v>-42.155999999999999</v>
+      </c>
+      <c r="E64">
+        <v>-50.616900000000001</v>
+      </c>
+      <c r="F64">
+        <v>-12.7387</v>
+      </c>
+      <c r="G64">
+        <v>21.2</v>
+      </c>
+      <c r="H64">
+        <v>137.89930363636299</v>
+      </c>
+      <c r="I64">
+        <v>0.33984752973342403</v>
+      </c>
+      <c r="J64">
+        <v>4.6164367404031198E-4</v>
+      </c>
+      <c r="K64">
+        <v>-4.7315675983402201</v>
+      </c>
+      <c r="M64">
+        <v>11</v>
+      </c>
+      <c r="N64" t="s">
+        <v>65</v>
+      </c>
+      <c r="O64">
+        <v>32.048008780000004</v>
+      </c>
+      <c r="P64">
+        <v>-12.117599999999999</v>
+      </c>
+      <c r="Q64">
+        <v>-32.759599999999999</v>
+      </c>
+      <c r="R64">
+        <v>-10.5222</v>
+      </c>
+      <c r="S64">
+        <v>31.164999999999999</v>
+      </c>
+      <c r="T64">
+        <v>26.061826163636301</v>
+      </c>
+      <c r="U64">
+        <v>3.49421402597403E-3</v>
+      </c>
+      <c r="V64">
+        <v>0.102308719121189</v>
+      </c>
+      <c r="W64">
+        <v>-1.40440534564541</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>44</v>
+      </c>
+      <c r="C65">
+        <v>103.9168198</v>
+      </c>
+      <c r="D65">
+        <v>-46.848999999999997</v>
+      </c>
+      <c r="E65">
+        <v>-63.137799999999999</v>
+      </c>
+      <c r="F65">
+        <v>-7.4077000000000002</v>
+      </c>
+      <c r="G65">
+        <v>23.696000000000002</v>
+      </c>
+      <c r="H65">
+        <v>91.397108909090903</v>
+      </c>
+      <c r="I65">
+        <v>0.19999130498974699</v>
+      </c>
+      <c r="J65">
+        <v>1.1520751282908801E-3</v>
+      </c>
+      <c r="K65">
+        <v>-4.1681898681317398</v>
+      </c>
+      <c r="N65" t="s">
+        <v>91</v>
+      </c>
+      <c r="O65">
+        <v>113.905233</v>
+      </c>
+      <c r="P65">
+        <v>-36.766300000000001</v>
+      </c>
+      <c r="Q65">
+        <v>-45.634399999999999</v>
+      </c>
+      <c r="R65">
+        <v>-13.468999999999999</v>
+      </c>
+      <c r="S65">
+        <v>22.335999999999999</v>
+      </c>
+      <c r="T65">
+        <v>100.477484545454</v>
+      </c>
+      <c r="U65">
+        <v>0.227300705399863</v>
+      </c>
+      <c r="V65">
+        <v>9.4563328159089305E-4</v>
+      </c>
+      <c r="W65">
+        <v>-4.2898347578318896</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>6</v>
+      </c>
+      <c r="B66" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66">
+        <v>76.922618049999997</v>
+      </c>
+      <c r="D66">
+        <v>-7.9169700000000001</v>
+      </c>
+      <c r="E66">
+        <v>-29.916499999999999</v>
+      </c>
+      <c r="F66">
+        <v>6.3299999999999995E-2</v>
+      </c>
+      <c r="G66">
+        <v>21.936</v>
+      </c>
+      <c r="H66">
+        <v>66.856925500000003</v>
+      </c>
+      <c r="I66">
+        <v>0.126186242105263</v>
+      </c>
+      <c r="J66">
+        <v>2.1783529604257799E-3</v>
+      </c>
+      <c r="K66">
+        <v>-3.7757748396099502</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>7</v>
+      </c>
+      <c r="B67" t="s">
+        <v>56</v>
+      </c>
+      <c r="C67">
+        <v>38.95720944</v>
+      </c>
+      <c r="D67">
+        <v>-18.024000000000001</v>
+      </c>
+      <c r="E67">
+        <v>-36.443100000000001</v>
+      </c>
+      <c r="F67">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="G67">
+        <v>18.408000000000001</v>
+      </c>
+      <c r="H67">
+        <v>32.342917672727197</v>
+      </c>
+      <c r="I67">
+        <v>2.2384714805194699E-2</v>
+      </c>
+      <c r="J67">
+        <v>1.5370461294637599E-2</v>
+      </c>
+      <c r="K67">
+        <v>-2.5721231587253102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>9</v>
+      </c>
+      <c r="B68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68">
+        <v>37.573075000000003</v>
+      </c>
+      <c r="D68">
+        <v>-24.5886</v>
+      </c>
+      <c r="E68">
+        <v>-46.728299999999997</v>
+      </c>
+      <c r="F68">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="G68">
+        <v>21.646999999999998</v>
+      </c>
+      <c r="H68">
+        <v>31.084613636363599</v>
+      </c>
+      <c r="I68">
+        <v>1.86003417634996E-2</v>
+      </c>
+      <c r="J68">
+        <v>1.8641179206052499E-2</v>
+      </c>
+      <c r="K68">
+        <v>-2.45327487734331</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>11</v>
+      </c>
+      <c r="B69" t="s">
+        <v>65</v>
+      </c>
+      <c r="C69">
+        <v>32.048008780000004</v>
+      </c>
+      <c r="D69">
+        <v>-12.117599999999999</v>
+      </c>
+      <c r="E69">
+        <v>-32.759599999999999</v>
+      </c>
+      <c r="F69">
+        <v>-10.5222</v>
+      </c>
+      <c r="G69">
+        <v>31.164999999999999</v>
+      </c>
+      <c r="H69">
+        <v>26.061826163636301</v>
+      </c>
+      <c r="I69">
+        <v>3.49421402597403E-3</v>
+      </c>
+      <c r="J69">
+        <v>0.102308719121189</v>
+      </c>
+      <c r="K69">
+        <v>-1.40440534564541</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>106</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72" t="s">
+        <v>10</v>
+      </c>
+      <c r="H72" t="s">
+        <v>19</v>
+      </c>
+      <c r="I72" t="s">
+        <v>20</v>
+      </c>
+      <c r="J72" t="s">
+        <v>21</v>
+      </c>
+      <c r="K72" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>0</v>
+      </c>
+      <c r="B73" t="s">
+        <v>107</v>
+      </c>
+      <c r="C73">
+        <v>39.726865452189699</v>
+      </c>
+      <c r="D73">
+        <v>-18.1389</v>
+      </c>
+      <c r="E73">
+        <v>-36.149700000000003</v>
+      </c>
+      <c r="F73">
+        <v>5.0800000000009497E-2</v>
+      </c>
+      <c r="G73">
+        <v>17.96</v>
+      </c>
+      <c r="H73">
+        <v>33.042604956536003</v>
+      </c>
+      <c r="I73">
+        <v>2.4489037463266399E-2</v>
+      </c>
+      <c r="J73">
+        <v>1.3989271330261101E-2</v>
+      </c>
+      <c r="K73">
+        <v>-2.6301268021156901</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>2</v>
+      </c>
+      <c r="B74" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74">
+        <v>53.989196811001698</v>
+      </c>
+      <c r="D74">
+        <v>-21.300599999999999</v>
+      </c>
+      <c r="E74">
+        <v>-44.918700000000001</v>
+      </c>
+      <c r="F74">
+        <v>0.201399999999992</v>
+      </c>
+      <c r="G74">
+        <v>23.417000000000002</v>
+      </c>
+      <c r="H74">
+        <v>46.008360737274202</v>
+      </c>
+      <c r="I74">
+        <v>6.3483791691050395E-2</v>
+      </c>
+      <c r="J74">
+        <v>4.9735929537687799E-3</v>
+      </c>
+      <c r="K74">
+        <v>-3.2671951829985</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>50</v>
+      </c>
+      <c r="C75">
+        <v>76.922618049999997</v>
+      </c>
+      <c r="D75">
+        <v>-7.9169700000000001</v>
+      </c>
+      <c r="E75">
+        <v>-29.916499999999999</v>
+      </c>
+      <c r="F75">
+        <v>6.3299999999999995E-2</v>
+      </c>
+      <c r="G75">
+        <v>21.936</v>
+      </c>
+      <c r="H75">
+        <v>66.856925500000003</v>
+      </c>
+      <c r="I75">
+        <v>0.126186242105263</v>
+      </c>
+      <c r="J75">
+        <v>2.1783529604257799E-3</v>
+      </c>
+      <c r="K75">
+        <v>-3.7757748396099502</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76">
+        <v>38.95720944</v>
+      </c>
+      <c r="D76">
+        <v>-18.024000000000001</v>
+      </c>
+      <c r="E76">
+        <v>-36.443100000000001</v>
+      </c>
+      <c r="F76">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="G76">
+        <v>18.408000000000001</v>
+      </c>
+      <c r="H76">
+        <v>32.342917672727197</v>
+      </c>
+      <c r="I76">
+        <v>2.2384714805194699E-2</v>
+      </c>
+      <c r="J76">
+        <v>1.5370461294637599E-2</v>
+      </c>
+      <c r="K76">
+        <v>-2.5721231587253102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>9</v>
+      </c>
+      <c r="B77" t="s">
+        <v>61</v>
+      </c>
+      <c r="C77">
+        <v>37.573075000000003</v>
+      </c>
+      <c r="D77">
+        <v>-24.5886</v>
+      </c>
+      <c r="E77">
+        <v>-46.728299999999997</v>
+      </c>
+      <c r="F77">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="G77">
+        <v>21.646999999999998</v>
+      </c>
+      <c r="H77">
+        <v>31.084613636363599</v>
+      </c>
+      <c r="I77">
+        <v>1.86003417634996E-2</v>
+      </c>
+      <c r="J77">
+        <v>1.8641179206052499E-2</v>
+      </c>
+      <c r="K77">
+        <v>-2.45327487734331</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>70</v>
+      </c>
+      <c r="C78">
+        <v>102.585914</v>
+      </c>
+      <c r="D78">
+        <v>-22.721900000000002</v>
+      </c>
+      <c r="E78">
+        <v>-43.788499999999999</v>
+      </c>
+      <c r="F78">
+        <v>0.12820000000000001</v>
+      </c>
+      <c r="G78">
+        <v>20.939</v>
+      </c>
+      <c r="H78">
+        <v>90.187194545454503</v>
+      </c>
+      <c r="I78">
+        <v>0.19635246479835899</v>
+      </c>
+      <c r="J78">
+        <v>1.1841245290178E-3</v>
+      </c>
+      <c r="K78">
+        <v>-4.1512866081039501</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>76</v>
+      </c>
+      <c r="C79">
+        <v>66.002636190000004</v>
+      </c>
+      <c r="D79">
+        <v>-19.871200000000002</v>
+      </c>
+      <c r="E79">
+        <v>-34.215200000000003</v>
+      </c>
+      <c r="F79">
+        <v>0.1971</v>
+      </c>
+      <c r="G79">
+        <v>14.147</v>
+      </c>
+      <c r="H79">
+        <v>56.929669263636299</v>
+      </c>
+      <c r="I79">
+        <v>9.6329832371838606E-2</v>
+      </c>
+      <c r="J79">
+        <v>3.0518387775783501E-3</v>
+      </c>
+      <c r="K79">
+        <v>-3.5680641155014499</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80">
+        <v>81.137700100000004</v>
+      </c>
+      <c r="D80">
+        <v>-14.2117</v>
+      </c>
+      <c r="E80">
+        <v>-44.609000000000002</v>
+      </c>
+      <c r="F80">
+        <v>0.36549999999999999</v>
+      </c>
+      <c r="G80">
+        <v>30.032</v>
+      </c>
+      <c r="H80">
+        <v>70.688818272727204</v>
+      </c>
+      <c r="I80">
+        <v>0.13771073164729999</v>
+      </c>
+      <c r="J80">
+        <v>1.94375121264627E-3</v>
+      </c>
+      <c r="K80">
+        <v>-3.8459712841690199</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>86</v>
+      </c>
+      <c r="C81">
+        <v>71.355192889999998</v>
+      </c>
+      <c r="D81">
+        <v>-17.953700000000001</v>
+      </c>
+      <c r="E81">
+        <v>-42.442799999999998</v>
+      </c>
+      <c r="F81">
+        <v>7.1832000000000003</v>
+      </c>
+      <c r="G81">
+        <v>17.306000000000001</v>
+      </c>
+      <c r="H81">
+        <v>61.795629899999902</v>
+      </c>
+      <c r="I81">
+        <v>0.110964300451127</v>
+      </c>
+      <c r="J81">
+        <v>2.5642338109576699E-3</v>
+      </c>
+      <c r="K81">
+        <v>-3.6753057764203998</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>96</v>
+      </c>
+      <c r="C82">
+        <v>44.477319909999999</v>
+      </c>
+      <c r="D82">
+        <v>-18.429099999999998</v>
+      </c>
+      <c r="E82">
+        <v>-40.478200000000001</v>
+      </c>
+      <c r="F82">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G82">
+        <v>21.965</v>
+      </c>
+      <c r="H82">
+        <v>37.361199918181804</v>
+      </c>
+      <c r="I82">
+        <v>3.7477292987012897E-2</v>
+      </c>
+      <c r="J82">
+        <v>8.8993083428196007E-3</v>
+      </c>
+      <c r="K82">
+        <v>-2.9087686362602199</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>100</v>
+      </c>
+      <c r="C83">
+        <v>88.949867569999995</v>
+      </c>
+      <c r="D83">
+        <v>-23.184699999999999</v>
+      </c>
+      <c r="E83">
+        <v>-45.356900000000003</v>
+      </c>
+      <c r="F83">
+        <v>7.14</v>
+      </c>
+      <c r="G83">
+        <v>15.032999999999999</v>
+      </c>
+      <c r="H83">
+        <v>77.790788699999993</v>
+      </c>
+      <c r="I83">
+        <v>0.159070041203007</v>
+      </c>
+      <c r="J83">
+        <v>1.60041921465234E-3</v>
+      </c>
+      <c r="K83">
+        <v>-3.9656996394062101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>